<commit_message>
add: pwsh: import a table by name using `ImportExcel`
</commit_message>
<xml_diff>
--- a/pwsh/Excel/Import-NamedTableRanges-NotWorksheets/Example.xlsx
+++ b/pwsh/Excel/Import-NamedTableRanges-NotWorksheets/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data\2025\GitRepos.🐒\TinyBits\pwsh\Excel\Import-NamedTableRanges-NotWorksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AE7A56-27C7-4C97-BE99-39055DD0E1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB390B93-789E-4E0D-901B-9D0BFCB80F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9390" yWindow="1965" windowWidth="25575" windowHeight="17610" activeTab="1" xr2:uid="{0AA8AF1B-DAFE-4E6F-AA59-6030ACB775A5}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="RawList" sheetId="1" r:id="rId1"/>
     <sheet name="OffsetTable" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -45,6 +45,12 @@
     <t>Species</t>
   </si>
   <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Hawk</t>
+  </si>
+  <si>
     <t>Hubert</t>
   </si>
   <si>
@@ -73,19 +79,14 @@
   </si>
   <si>
     <t>Mouse</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Hawk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -115,7 +116,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,64 +584,65 @@
     <col min="1" max="2" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" s="0" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -652,7 +654,7 @@
   <dimension ref="M11:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -660,64 +662,65 @@
     <col min="14" max="14" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M11" t="s">
+    <row r="11">
+      <c r="M11" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M12" t="s">
+    <row r="12">
+      <c r="M12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="M13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="M14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="M15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="M16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="M17" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N17" s="0" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M14" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M15" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M16" t="s">
-        <v>8</v>
-      </c>
-      <c r="N16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N17" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>